<commit_message>
plotted both simbrief and flightaware
</commit_message>
<xml_diff>
--- a/PHX-LV/Simbrief_Comparisons/PHX_LAS_022624_2328.xlsx
+++ b/PHX-LV/Simbrief_Comparisons/PHX_LAS_022624_2328.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashle\Documents\GitHub\Honeywell-Project\PHX-LV\Simbrief_Comparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360E4EBA-9EB5-4E97-8F2C-FAE30151304C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E241B0-70E8-4BA6-8372-A3FBE4A81ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4D786241-E327-4B8B-89F0-DAB4D98E1050}"/>
   </bookViews>
@@ -1399,7 +1399,7 @@
   <dimension ref="A1:J131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>